<commit_message>
2020.11.9 更新 《Effective Java（第3版）》笔记.md
</commit_message>
<xml_diff>
--- a/学习笔记存储文件夹/知识点原材料/日常学习时间记录.xlsx
+++ b/学习笔记存储文件夹/知识点原材料/日常学习时间记录.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\learning-platform\学习笔记存储文件夹\知识点原材料\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="12990"/>
+    <workbookView windowWidth="13590" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>日期</t>
   </si>
@@ -97,6 +92,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>第1条</t>
     </r>
     <r>
@@ -104,20 +106,27 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 用静态工厂方法替代构造器</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第2条 遇到多个构造器参数时要考虑使用构建器 到 第5条 优先考虑依赖注入来引用资源</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,30 +135,345 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -157,11 +481,253 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -173,30 +739,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -454,26 +1058,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="32.125" customWidth="1"/>
     <col min="6" max="6" width="42.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +1097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>44137</v>
       </c>
@@ -501,300 +1105,300 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>0.97916666666666696</v>
+        <v>0.979166666666667</v>
       </c>
       <c r="D2" s="3">
-        <v>0.99652777777777801</v>
+        <v>0.996527777777778</v>
       </c>
       <c r="E2" s="3">
         <f>D2-C2</f>
-        <v>1.7361111111111049E-2</v>
+        <v>0.017361111111111</v>
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
         <v>44138</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.99722222222222201</v>
+        <v>0.997222222222222</v>
       </c>
       <c r="D3" s="3">
-        <v>1.7361111111111101E-2</v>
+        <v>0.0173611111111111</v>
       </c>
       <c r="E3" s="3">
-        <v>2.0833333333333301E-2</v>
+        <v>0.0208333333333333</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="3">
-        <v>0.59027777777777801</v>
+        <v>0.590277777777778</v>
       </c>
       <c r="D4" s="3">
-        <v>0.61458333333333304</v>
+        <v>0.614583333333333</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E16" si="0">D4-C4</f>
-        <v>2.4305555555555025E-2</v>
+        <f t="shared" ref="E4:E19" si="0">D4-C4</f>
+        <v>0.024305555555555</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>0.62916666666666698</v>
+        <v>0.629166666666667</v>
       </c>
       <c r="D5" s="3">
-        <v>0.72083333333333299</v>
+        <v>0.720833333333333</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>9.1666666666666008E-2</v>
+        <v>0.091666666666666</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
         <v>44139</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3">
-        <v>0.65277777777777801</v>
+        <v>0.652777777777778</v>
       </c>
       <c r="D6" s="3">
-        <v>0.75277777777777799</v>
+        <v>0.752777777777778</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="3">
-        <v>0.78611111111111098</v>
+        <v>0.786111111111111</v>
       </c>
       <c r="D7" s="3">
-        <v>0.82777777777777795</v>
+        <v>0.827777777777778</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666963E-2</v>
+        <v>0.041666666666667</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
         <v>44140</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3">
-        <v>0.42569444444444399</v>
+        <v>0.425694444444444</v>
       </c>
       <c r="D8" s="3">
-        <v>0.48819444444444399</v>
+        <v>0.488194444444444</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0.0625</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3">
-        <v>0.61805555555555602</v>
+        <v>0.618055555555556</v>
       </c>
       <c r="D9" s="3">
-        <v>0.67222222222222205</v>
+        <v>0.672222222222222</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>5.416666666666603E-2</v>
+        <v>0.054166666666666</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="3">
-        <v>0.68333333333333302</v>
+        <v>0.683333333333333</v>
       </c>
       <c r="D10" s="3">
-        <v>0.75416666666666698</v>
+        <v>0.754166666666667</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>7.083333333333397E-2</v>
+        <v>0.070833333333334</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="3">
         <v>0.781944444444444</v>
       </c>
       <c r="D11" s="3">
-        <v>0.80277777777777803</v>
+        <v>0.802777777777778</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>2.0833333333334036E-2</v>
+        <v>0.020833333333334</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3">
-        <v>0.80486111111111103</v>
+        <v>0.804861111111111</v>
       </c>
       <c r="D12" s="3">
-        <v>0.83333333333333304</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>2.847222222222201E-2</v>
+        <v>0.028472222222222</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
         <v>44141</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="3">
         <v>0.422222222222222</v>
       </c>
       <c r="D13" s="3">
-        <v>0.50347222222222199</v>
+        <v>0.503472222222222</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="0"/>
-        <v>8.1249999999999989E-2</v>
+        <v>0.08125</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="3">
-        <v>0.60694444444444395</v>
+        <v>0.606944444444444</v>
       </c>
       <c r="D14" s="3">
-        <v>0.73402777777777795</v>
+        <v>0.734027777777778</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="0"/>
-        <v>0.12708333333333399</v>
+        <v>0.127083333333334</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="3">
-        <v>0.80416666666666703</v>
+        <v>0.804166666666667</v>
       </c>
       <c r="D15" s="3">
         <v>0.8125</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="0"/>
-        <v>8.3333333333329707E-3</v>
+        <v>0.00833333333333297</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
         <v>44142</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3">
-        <v>0.70277777777777795</v>
+        <v>0.702777777777778</v>
       </c>
       <c r="D16" s="3">
-        <v>0.75138888888888899</v>
+        <v>0.751388888888889</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>4.8611111111111049E-2</v>
+        <v>0.048611111111111</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="3">
-        <v>0.77152777777777803</v>
+        <v>0.771527777777778</v>
       </c>
       <c r="D17" s="3">
-        <v>0.82291666666666696</v>
+        <v>0.822916666666667</v>
       </c>
       <c r="E17" s="3">
-        <f>D17-C17</f>
-        <v>5.1388888888888928E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.0513888888888889</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>44143</v>
       </c>
@@ -802,61 +1406,78 @@
         <v>6</v>
       </c>
       <c r="C18" s="3">
-        <v>0.93055555555555547</v>
+        <v>0.930555555555555</v>
       </c>
       <c r="D18" s="3">
-        <v>0.9916666666666667</v>
+        <v>0.991666666666667</v>
       </c>
       <c r="E18" s="3">
-        <f>D18-C18</f>
-        <v>6.1111111111111227E-2</v>
-      </c>
-      <c r="F18" s="8" t="s">
+        <f t="shared" si="0"/>
+        <v>0.061111111111112</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>44144</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.404861111111111</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.509722222222222</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.104861111111111</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="2"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="2"/>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:1">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" s="2"/>
     </row>
   </sheetData>
@@ -872,8 +1493,8 @@
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="B16:B17"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>